<commit_message>
Somthing new added, dont know
</commit_message>
<xml_diff>
--- a/Credentials/Scalping - Virtual.xlsx
+++ b/Credentials/Scalping - Virtual.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CFD497-0249-4077-91D2-100FFEFBB747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="22968" windowHeight="7116"/>
+    <workbookView xWindow="4067" yWindow="1333" windowWidth="21033" windowHeight="10094" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nifty" sheetId="1" r:id="rId1"/>
     <sheet name="Bank-Nifty" sheetId="2" r:id="rId2"/>
     <sheet name="Sensex" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +24,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="96">
   <si>
     <t>Points</t>
   </si>
@@ -265,55 +268,67 @@
     <t>BSE_FO|887010</t>
   </si>
   <si>
+    <t>Order Quantity : 510</t>
+  </si>
+  <si>
+    <t>Synthetic ATM Strike : 59900</t>
+  </si>
+  <si>
+    <t>Bank-Nifty SPOT : 59757.4</t>
+  </si>
+  <si>
+    <t>Days to Expiry : 25 (Tuesday)</t>
+  </si>
+  <si>
+    <t>Bank-Nifty : Mohit Sharma (Live Virtual Trade) | Today : 02-01-2026 / Friday | 09:12:53 AM</t>
+  </si>
+  <si>
+    <t>Synthetic ATM Strike : 85300</t>
+  </si>
+  <si>
+    <t>Sensex SPOT : 85259.36</t>
+  </si>
+  <si>
+    <t>Days to Expiry : 6 (Thursday)</t>
+  </si>
+  <si>
+    <t>Sensex : Mohit Sharma (Live Virtual Trade) | Today : 02-01-2026 / Friday | 09:12:56 AM</t>
+  </si>
+  <si>
+    <t>Days to Expiry : 4 (Tuesday)</t>
+  </si>
+  <si>
     <t>Order Quantity : 1755</t>
   </si>
   <si>
-    <t>Order Quantity : 510</t>
-  </si>
-  <si>
-    <t>Synthetic ATM Strike : 59900</t>
-  </si>
-  <si>
-    <t>Bank-Nifty SPOT : 59757.4</t>
-  </si>
-  <si>
-    <t>Days to Expiry : 25 (Tuesday)</t>
-  </si>
-  <si>
-    <t>Bank-Nifty : Mohit Sharma (Live Virtual Trade) | Today : 02-01-2026 / Friday | 09:12:53 AM</t>
-  </si>
-  <si>
-    <t>Synthetic ATM Strike : 85300</t>
-  </si>
-  <si>
-    <t>Sensex SPOT : 85259.36</t>
-  </si>
-  <si>
-    <t>Days to Expiry : 6 (Thursday)</t>
-  </si>
-  <si>
-    <t>Sensex : Mohit Sharma (Live Virtual Trade) | Today : 02-01-2026 / Friday | 09:12:56 AM</t>
-  </si>
-  <si>
-    <t>Days to Expiry : 6 (Tuesday)</t>
-  </si>
-  <si>
-    <t>Synthetic ATM Strike : 25800</t>
-  </si>
-  <si>
-    <t>NSE_FO|47617</t>
-  </si>
-  <si>
-    <t>Nifty : Mohit Sharma (Live Virtual Trade) | Today : 14-01-2026 / Wednesday | 12:34:52 PM</t>
-  </si>
-  <si>
-    <t>Nifty SPOT : 25765.85</t>
+    <t>NSE_FO|58689</t>
+  </si>
+  <si>
+    <t>NSE_FO|58690</t>
+  </si>
+  <si>
+    <t>Total Profit</t>
+  </si>
+  <si>
+    <t>Synthetic ATM Strike : 25200</t>
+  </si>
+  <si>
+    <t>Position Closed</t>
+  </si>
+  <si>
+    <t>SELL</t>
+  </si>
+  <si>
+    <t>Nifty : Lalit Sharma (Live Virtual Trade) | Today : 23-01-2026 / Friday | 12:14:00 PM</t>
+  </si>
+  <si>
+    <t>Nifty SPOT : 25187.75</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
@@ -1162,7 +1177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1297,8 +1312,164 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1306,164 +1477,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1843,61 +1863,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.41015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.64453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1171875" customWidth="1"/>
+    <col min="10" max="10" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1171875" customWidth="1"/>
+    <col min="12" max="12" width="8.87890625" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.41015625" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="120"/>
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="77"/>
+      <c r="B1" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="83"/>
+      <c r="D1" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="80"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="96"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="121"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="100"/>
+    </row>
+    <row r="2" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="78"/>
       <c r="B2" s="44" t="s">
         <v>59</v>
       </c>
@@ -1913,47 +1933,47 @@
       <c r="F2" s="69">
         <v>0</v>
       </c>
-      <c r="G2" s="108"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="41" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="34">
-        <v>29659.499999999913</v>
+        <v>861.24999999999545</v>
       </c>
       <c r="J2" s="42" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="43">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L2" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="97" t="s">
+      <c r="M2" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="98"/>
-      <c r="O2" s="99"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="121"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="125"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A3" s="78"/>
       <c r="B3" s="44" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8">
         <v>27</v>
       </c>
-      <c r="D3" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="108"/>
+      <c r="D3" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="86"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="4">
-        <v>-10036</v>
+        <v>-4558</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>8</v>
@@ -1962,59 +1982,59 @@
         <v>5</v>
       </c>
       <c r="L3" s="65">
-        <v>25500</v>
-      </c>
-      <c r="M3" s="74" t="s">
+        <v>25100</v>
+      </c>
+      <c r="M3" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="75" t="s">
+      <c r="N3" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="76" t="s">
+      <c r="O3" s="128" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="78"/>
       <c r="B4" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="56">
-        <v>46042</v>
-      </c>
-      <c r="D4" s="118" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="108"/>
+        <v>46049</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="46" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="6">
-        <v>19623.499999999909</v>
+        <v>-3696.7500000000045</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K4" s="45">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="L4" s="65">
-        <v>25550</v>
+        <v>25150</v>
       </c>
       <c r="M4" s="12">
-        <v>7406.75</v>
+        <v>7679.75</v>
       </c>
       <c r="N4" s="7">
-        <v>8440.25</v>
+        <v>6496.75</v>
       </c>
       <c r="O4" s="13">
-        <v>15847</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="121"/>
+        <v>14235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="78"/>
       <c r="B5" s="51" t="s">
         <v>53</v>
       </c>
@@ -2024,83 +2044,83 @@
       <c r="D5" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="124"/>
-      <c r="G5" s="108"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="44" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>16.899999999999949</v>
+        <v>12.25</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>63</v>
       </c>
       <c r="K5" s="48">
-        <v>0.78259999999999996</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="L5" s="65">
-        <v>25600</v>
+        <v>25200</v>
       </c>
       <c r="M5" s="20">
         <f>M4*$C$3</f>
-        <v>199982.25</v>
+        <v>207353.25</v>
       </c>
       <c r="N5" s="21">
         <f t="shared" ref="N5:O5" si="0">N4*$C$3</f>
-        <v>227886.75</v>
+        <v>175412.25</v>
       </c>
       <c r="O5" s="22">
         <f t="shared" si="0"/>
-        <v>427869</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="121"/>
+        <v>384345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="78"/>
       <c r="B6" s="50">
-        <v>114.2</v>
+        <v>118.1</v>
       </c>
       <c r="C6" s="52">
-        <v>25800</v>
+        <v>25200</v>
       </c>
       <c r="D6" s="39">
-        <v>129.35</v>
+        <v>100.45</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>57</v>
       </c>
       <c r="F6" s="38">
         <f>B6-D6+C6</f>
-        <v>25784.85</v>
-      </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="84" t="s">
+        <v>25217.65</v>
+      </c>
+      <c r="G6" s="112"/>
+      <c r="H6" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="85"/>
+      <c r="I6" s="89"/>
       <c r="J6" s="63">
-        <v>32295.749999999913</v>
+        <v>6459.4999999999845</v>
       </c>
       <c r="K6" s="64">
-        <v>-12672.250000000005</v>
+        <v>-10156.249999999989</v>
       </c>
       <c r="L6" s="65">
-        <v>25650</v>
+        <v>25250</v>
       </c>
       <c r="M6" s="15">
-        <v>-419</v>
+        <v>-430</v>
       </c>
       <c r="N6" s="16">
-        <v>-471</v>
+        <v>-376</v>
       </c>
       <c r="O6" s="17">
-        <v>-891</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="121"/>
+        <v>-807</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="78"/>
       <c r="B7" s="53">
         <v>0</v>
       </c>
@@ -2110,33 +2130,33 @@
       <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="106" t="s">
+      <c r="E7" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="107"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="103" t="s">
+      <c r="F7" s="111"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="105"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="109"/>
       <c r="L7" s="65">
-        <v>25700</v>
-      </c>
-      <c r="M7" s="97" t="s">
+        <v>25300</v>
+      </c>
+      <c r="M7" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="98"/>
-      <c r="O7" s="99"/>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="121"/>
+      <c r="N7" s="124"/>
+      <c r="O7" s="125"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="78"/>
       <c r="B8" s="57"/>
       <c r="C8" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="96" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="27" t="s">
@@ -2145,121 +2165,121 @@
       <c r="F8" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="108"/>
+      <c r="G8" s="112"/>
       <c r="H8" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="77">
+      <c r="I8" s="121">
         <v>1</v>
       </c>
-      <c r="J8" s="102" t="s">
+      <c r="J8" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="100"/>
+      <c r="K8" s="104"/>
       <c r="L8" s="65">
-        <v>25750</v>
-      </c>
-      <c r="M8" s="74" t="s">
+        <v>25350</v>
+      </c>
+      <c r="M8" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="76" t="s">
+      <c r="O8" s="128" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A9" s="78"/>
       <c r="B9" s="59" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="93"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="70" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="71">
         <v>1</v>
       </c>
-      <c r="G9" s="108"/>
+      <c r="G9" s="112"/>
       <c r="H9" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="72">
+      <c r="I9" s="121">
         <v>0</v>
       </c>
-      <c r="J9" s="102"/>
-      <c r="K9" s="100"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="104"/>
       <c r="L9" s="65">
-        <v>25800</v>
+        <v>25400</v>
       </c>
       <c r="M9" s="12">
-        <v>182187.655</v>
+        <v>191401.27499999999</v>
       </c>
       <c r="N9" s="7">
-        <v>188724.185</v>
+        <v>176081.88</v>
       </c>
       <c r="O9" s="13">
-        <v>222362.40000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="121"/>
+        <v>224282.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="78"/>
       <c r="B10" s="59" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="93"/>
+      <c r="D10" s="97"/>
       <c r="E10" s="29" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="108"/>
-      <c r="H10" s="129" t="s">
+      <c r="G10" s="112"/>
+      <c r="H10" s="120" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="117"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="74"/>
       <c r="L10" s="65">
-        <v>25850</v>
+        <v>25450</v>
       </c>
       <c r="M10" s="23">
         <f>M9*$C$3</f>
-        <v>4919066.6849999996</v>
+        <v>5167834.4249999998</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" ref="N10:O10" si="1">N9*$C$3</f>
-        <v>5095552.9950000001</v>
+        <v>4754210.76</v>
       </c>
       <c r="O10" s="25">
         <f t="shared" si="1"/>
-        <v>6003784.8000000007</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="121"/>
+        <v>6055627.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="78"/>
       <c r="B11" s="59" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="31" t="s">
         <v>67</v>
       </c>
       <c r="F11" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="108"/>
+      <c r="G11" s="112"/>
       <c r="H11" s="10">
         <v>0</v>
       </c>
@@ -2269,105 +2289,105 @@
       <c r="J11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="100" t="s">
+      <c r="K11" s="104" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="65">
-        <v>25900</v>
-      </c>
-      <c r="M11" s="89" t="s">
+        <v>25500</v>
+      </c>
+      <c r="M11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="90"/>
-      <c r="O11" s="91"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="121"/>
+      <c r="N11" s="94"/>
+      <c r="O11" s="95"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A12" s="78"/>
       <c r="B12" s="59" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="93"/>
+      <c r="D12" s="97"/>
       <c r="E12" s="31" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="108"/>
+      <c r="G12" s="112"/>
       <c r="H12" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="72">
+      <c r="I12" s="121">
         <v>0</v>
       </c>
-      <c r="J12" s="72">
+      <c r="J12" s="121">
         <v>0</v>
       </c>
-      <c r="K12" s="100"/>
+      <c r="K12" s="104"/>
       <c r="L12" s="65">
-        <v>25950</v>
-      </c>
-      <c r="M12" s="109" t="s">
-        <v>69</v>
-      </c>
-      <c r="N12" s="110"/>
-      <c r="O12" s="111"/>
-    </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="122"/>
+        <v>25550</v>
+      </c>
+      <c r="M12" s="129" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="114"/>
+      <c r="O12" s="115"/>
+    </row>
+    <row r="13" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="79"/>
       <c r="B13" s="61" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="94"/>
+      <c r="D13" s="98"/>
       <c r="E13" s="35" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="88"/>
+      <c r="G13" s="92"/>
       <c r="H13" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="73">
+      <c r="I13" s="122">
         <v>0</v>
       </c>
-      <c r="J13" s="73">
+      <c r="J13" s="122">
         <v>0</v>
       </c>
-      <c r="K13" s="101"/>
+      <c r="K13" s="105"/>
       <c r="L13" s="66">
-        <v>26000</v>
-      </c>
-      <c r="M13" s="112"/>
-      <c r="N13" s="113"/>
-      <c r="O13" s="114"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="86"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
+        <v>25600</v>
+      </c>
+      <c r="M13" s="116"/>
+      <c r="N13" s="117"/>
+      <c r="O13" s="118"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="90"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="92"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
+      <c r="O14" s="92"/>
       <c r="P14" s="18"/>
     </row>
-    <row r="15" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -2401,25 +2421,19 @@
       <c r="L15" t="s">
         <v>6</v>
       </c>
-      <c r="M15" t="s">
-        <v>4</v>
-      </c>
-      <c r="N15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="D16">
-        <v>25800</v>
+        <v>25200</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
@@ -2434,72 +2448,124 @@
         <v>1755</v>
       </c>
       <c r="I16">
-        <v>112.4</v>
+        <v>119.7</v>
       </c>
       <c r="J16" s="14">
-        <v>114.15</v>
+        <v>118</v>
       </c>
       <c r="K16">
-        <v>1.75</v>
+        <v>1.7000000000000028</v>
       </c>
       <c r="L16">
-        <v>3071.25</v>
-      </c>
-      <c r="M16">
-        <v>-418</v>
-      </c>
-      <c r="N16" s="2">
-        <v>2653.25</v>
-      </c>
+        <v>2983.500000000005</v>
+      </c>
+      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="M17" t="s">
-        <v>43</v>
-      </c>
-      <c r="N17" s="1">
-        <v>1.35E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>25200</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>65</v>
+      </c>
+      <c r="G17">
+        <v>27</v>
+      </c>
+      <c r="H17">
+        <v>1755</v>
+      </c>
+      <c r="I17">
+        <v>98.5</v>
+      </c>
+      <c r="J17">
+        <v>100.6</v>
+      </c>
+      <c r="K17">
+        <v>-2.0999999999999943</v>
+      </c>
+      <c r="L17">
+        <v>-3685.49999999999</v>
+      </c>
+      <c r="N17" s="130"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="M18" t="s">
+      <c r="J18">
+        <v>-0.39999999999999147</v>
+      </c>
+      <c r="K18" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18">
+        <v>-701.99999999998499</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="2">
+        <v>-806</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="2">
+        <v>-1507.999999999985</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="3">
-        <v>197262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J19" s="3"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J21" s="3"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J21" s="3">
+        <v>6055564.3200000003</v>
+      </c>
+      <c r="K21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="1">
+        <v>-1E-4</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E23" s="36"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="20">
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A1:A13"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H6:I6"/>
     <mergeCell ref="A14:O14"/>
     <mergeCell ref="M11:O11"/>
     <mergeCell ref="D8:D13"/>
@@ -2512,6 +2578,14 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G1:G13"/>
     <mergeCell ref="M12:O13"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A1:A13"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="K16:O16">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
@@ -2543,7 +2617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -2551,49 +2625,49 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" customWidth="1"/>
-    <col min="7" max="7" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1171875" customWidth="1"/>
+    <col min="7" max="7" width="3.3515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.87890625" customWidth="1"/>
+    <col min="10" max="10" width="14.3515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.87890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.52734375" customWidth="1"/>
+    <col min="13" max="13" width="11.3515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.64453125" customWidth="1"/>
+    <col min="15" max="15" width="11.3515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="120"/>
-      <c r="B1" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="80" t="s">
+    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="77"/>
+      <c r="B1" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="80"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="95" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="96"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="121"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="100"/>
+    </row>
+    <row r="2" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="78"/>
       <c r="B2" s="44" t="s">
         <v>60</v>
       </c>
@@ -2609,14 +2683,14 @@
       <c r="F2" s="69">
         <v>0</v>
       </c>
-      <c r="G2" s="108"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="41" t="str">
         <f>Nifty!H2</f>
         <v>Profit</v>
       </c>
       <c r="I2" s="34">
         <f>Nifty!I2</f>
-        <v>29659.499999999913</v>
+        <v>861.24999999999545</v>
       </c>
       <c r="J2" s="42" t="str">
         <f>Nifty!J2</f>
@@ -2624,38 +2698,38 @@
       </c>
       <c r="K2" s="43">
         <f>Nifty!K2</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L2" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="125" t="s">
+      <c r="M2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="126"/>
-      <c r="O2" s="127"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="121"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="103"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A3" s="78"/>
       <c r="B3" s="44" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="8">
         <v>17</v>
       </c>
-      <c r="D3" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="108"/>
+      <c r="D3" s="86" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="86"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="44" t="str">
         <f>Nifty!H3</f>
         <v>Brokerage</v>
       </c>
       <c r="I3" s="4">
         <f>Nifty!I3</f>
-        <v>-10036</v>
+        <v>-4558</v>
       </c>
       <c r="J3" s="5" t="str">
         <f>Nifty!J3</f>
@@ -2666,7 +2740,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="65">
-        <v>59300</v>
+        <v>58800</v>
       </c>
       <c r="M3" s="10" t="s">
         <v>2</v>
@@ -2678,27 +2752,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="78"/>
       <c r="B4" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="56">
         <v>46049</v>
       </c>
-      <c r="D4" s="118" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="108"/>
+      <c r="D4" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="46" t="str">
         <f>Nifty!H4</f>
         <v>Net Profit</v>
       </c>
       <c r="I4" s="6">
         <f>Nifty!I4</f>
-        <v>19623.499999999909</v>
+        <v>-3696.7500000000045</v>
       </c>
       <c r="J4" s="5" t="str">
         <f>Nifty!J4</f>
@@ -2706,10 +2780,10 @@
       </c>
       <c r="K4" s="45">
         <f>Nifty!K4</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="L4" s="65">
-        <v>59400</v>
+        <v>58900</v>
       </c>
       <c r="M4" s="12">
         <v>22386</v>
@@ -2721,8 +2795,8 @@
         <v>35791</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="78"/>
       <c r="B5" s="51" t="s">
         <v>2</v>
       </c>
@@ -2732,18 +2806,18 @@
       <c r="D5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="124"/>
-      <c r="G5" s="108"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="44" t="str">
         <f>Nifty!H5</f>
         <v>Points</v>
       </c>
       <c r="I5" s="4">
         <f>Nifty!I5</f>
-        <v>16.899999999999949</v>
+        <v>12.25</v>
       </c>
       <c r="J5" s="5" t="str">
         <f>Nifty!J5</f>
@@ -2751,10 +2825,10 @@
       </c>
       <c r="K5" s="48">
         <f>Nifty!K5</f>
-        <v>0.78259999999999996</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="L5" s="65">
-        <v>59500</v>
+        <v>59000</v>
       </c>
       <c r="M5" s="20">
         <f>M4*$C$3</f>
@@ -2769,13 +2843,13 @@
         <v>608447</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="78"/>
       <c r="B6" s="50">
         <v>684</v>
       </c>
       <c r="C6" s="52">
-        <v>59600</v>
+        <v>58900</v>
       </c>
       <c r="D6" s="39">
         <v>537.6</v>
@@ -2785,24 +2859,24 @@
       </c>
       <c r="F6" s="38">
         <f>B6-D6+C6</f>
-        <v>59746.400000000001</v>
-      </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="84" t="str">
+        <v>59046.400000000001</v>
+      </c>
+      <c r="G6" s="112"/>
+      <c r="H6" s="88" t="str">
         <f>Nifty!H6</f>
         <v>Positives &amp; Negatives</v>
       </c>
-      <c r="I6" s="85"/>
+      <c r="I6" s="89"/>
       <c r="J6" s="63">
         <f>Nifty!J6</f>
-        <v>32295.749999999913</v>
+        <v>6459.4999999999845</v>
       </c>
       <c r="K6" s="64">
         <f>Nifty!K6</f>
-        <v>-12672.250000000005</v>
+        <v>-10156.249999999989</v>
       </c>
       <c r="L6" s="65">
-        <v>59600</v>
+        <v>59100</v>
       </c>
       <c r="M6" s="15">
         <v>-731</v>
@@ -2814,8 +2888,8 @@
         <v>-1178</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="78"/>
       <c r="B7" s="53">
         <v>0</v>
       </c>
@@ -2825,35 +2899,35 @@
       <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="106" t="s">
+      <c r="E7" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="107"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="103" t="s">
+      <c r="F7" s="111"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="105"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="109"/>
       <c r="L7" s="65">
-        <v>59700</v>
-      </c>
-      <c r="M7" s="125" t="s">
+        <v>59200</v>
+      </c>
+      <c r="M7" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="126"/>
-      <c r="O7" s="127"/>
-    </row>
-    <row r="8" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="121"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="103"/>
+    </row>
+    <row r="8" spans="1:16" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="78"/>
       <c r="B8" s="57" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="96" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="27" t="s">
@@ -2862,19 +2936,19 @@
       <c r="F8" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="108"/>
+      <c r="G8" s="112"/>
       <c r="H8" s="44" t="s">
         <v>22</v>
       </c>
       <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="J8" s="102" t="s">
+      <c r="J8" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="100"/>
+      <c r="K8" s="104"/>
       <c r="L8" s="65">
-        <v>59800</v>
+        <v>59300</v>
       </c>
       <c r="M8" s="10" t="s">
         <v>2</v>
@@ -2886,32 +2960,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A9" s="78"/>
       <c r="B9" s="59" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="93"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="70" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="71">
         <v>0</v>
       </c>
-      <c r="G9" s="108"/>
+      <c r="G9" s="112"/>
       <c r="H9" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="8">
         <v>0</v>
       </c>
-      <c r="J9" s="102"/>
-      <c r="K9" s="100"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="104"/>
       <c r="L9" s="65">
-        <v>59900</v>
+        <v>59400</v>
       </c>
       <c r="M9" s="12">
         <v>273379.08499999996</v>
@@ -2923,30 +2997,30 @@
         <v>315220.14999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="78"/>
       <c r="B10" s="59" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="93"/>
+      <c r="D10" s="97"/>
       <c r="E10" s="29" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="108"/>
-      <c r="H10" s="115" t="s">
+      <c r="G10" s="112"/>
+      <c r="H10" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="117"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="74"/>
       <c r="L10" s="65">
-        <v>60000</v>
+        <v>59500</v>
       </c>
       <c r="M10" s="23">
         <f>M9*$C$3</f>
@@ -2961,22 +3035,22 @@
         <v>5358742.55</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="78"/>
       <c r="B11" s="59" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="31" t="s">
         <v>67</v>
       </c>
       <c r="F11" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="108"/>
+      <c r="G11" s="112"/>
       <c r="H11" s="10">
         <v>0</v>
       </c>
@@ -2986,34 +3060,34 @@
       <c r="J11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="100" t="s">
+      <c r="K11" s="104" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="65">
-        <v>60100</v>
-      </c>
-      <c r="M11" s="89" t="s">
+        <v>59600</v>
+      </c>
+      <c r="M11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="90"/>
-      <c r="O11" s="91"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="121"/>
+      <c r="N11" s="94"/>
+      <c r="O11" s="95"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A12" s="78"/>
       <c r="B12" s="59" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="93"/>
+      <c r="D12" s="97"/>
       <c r="E12" s="31" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="108"/>
+      <c r="G12" s="112"/>
       <c r="H12" s="44" t="s">
         <v>28</v>
       </c>
@@ -3023,32 +3097,32 @@
       <c r="J12" s="8">
         <v>0</v>
       </c>
-      <c r="K12" s="100"/>
+      <c r="K12" s="104"/>
       <c r="L12" s="65">
-        <v>60200</v>
-      </c>
-      <c r="M12" s="128" t="s">
+        <v>59700</v>
+      </c>
+      <c r="M12" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="N12" s="110"/>
-      <c r="O12" s="111"/>
-    </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="122"/>
+      <c r="N12" s="114"/>
+      <c r="O12" s="115"/>
+    </row>
+    <row r="13" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="79"/>
       <c r="B13" s="61" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="94"/>
+      <c r="D13" s="98"/>
       <c r="E13" s="35" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="88"/>
+      <c r="G13" s="92"/>
       <c r="H13" s="47" t="s">
         <v>29</v>
       </c>
@@ -3058,33 +3132,33 @@
       <c r="J13" s="33">
         <v>0</v>
       </c>
-      <c r="K13" s="101"/>
+      <c r="K13" s="105"/>
       <c r="L13" s="66">
-        <v>60300</v>
-      </c>
-      <c r="M13" s="112"/>
-      <c r="N13" s="113"/>
-      <c r="O13" s="114"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="86"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
+        <v>59800</v>
+      </c>
+      <c r="M13" s="116"/>
+      <c r="N13" s="117"/>
+      <c r="O13" s="118"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="90"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
+      <c r="O14" s="92"/>
       <c r="P14" s="19"/>
     </row>
-    <row r="15" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -3125,7 +3199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3169,7 +3243,7 @@
         <v>229.99999999998647</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3180,7 +3254,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3191,15 +3265,11 @@
         <v>311542</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.5">
       <c r="L21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J8:K9"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="M12:O13"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="D3:F3"/>
@@ -3216,6 +3286,10 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="H1:O1"/>
     <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J8:K9"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="M12:O13"/>
   </mergeCells>
   <conditionalFormatting sqref="L17:L21">
     <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
@@ -3238,7 +3312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -3246,48 +3320,48 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.3515625" customWidth="1"/>
+    <col min="2" max="2" width="18.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.41015625" customWidth="1"/>
+    <col min="7" max="7" width="3.3515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.41015625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="7.64453125" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.52734375" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="120"/>
-      <c r="B1" s="78" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="80" t="s">
+    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="77"/>
+      <c r="B1" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="80"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="95" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="96"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="121"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="100"/>
+    </row>
+    <row r="2" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="78"/>
       <c r="B2" s="44" t="s">
         <v>61</v>
       </c>
@@ -3303,14 +3377,14 @@
       <c r="F2" s="69">
         <v>0</v>
       </c>
-      <c r="G2" s="108"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="41" t="str">
         <f>Nifty!H2</f>
         <v>Profit</v>
       </c>
       <c r="I2" s="34">
         <f>Nifty!I2</f>
-        <v>29659.499999999913</v>
+        <v>861.24999999999545</v>
       </c>
       <c r="J2" s="42" t="str">
         <f>Nifty!J2</f>
@@ -3318,38 +3392,38 @@
       </c>
       <c r="K2" s="43">
         <f>Nifty!K2</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L2" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="125" t="s">
+      <c r="M2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="126"/>
-      <c r="O2" s="127"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="121"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="103"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A3" s="78"/>
       <c r="B3" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="108"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="44" t="str">
         <f>Nifty!H3</f>
         <v>Brokerage</v>
       </c>
       <c r="I3" s="4">
         <f>Nifty!I3</f>
-        <v>-10036</v>
+        <v>-4558</v>
       </c>
       <c r="J3" s="5" t="str">
         <f>Nifty!J3</f>
@@ -3360,7 +3434,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="65">
-        <v>83100</v>
+        <v>82000</v>
       </c>
       <c r="M3" s="10" t="s">
         <v>2</v>
@@ -3372,27 +3446,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="78"/>
       <c r="B4" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="56">
         <v>46030</v>
       </c>
-      <c r="D4" s="118" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="108"/>
+      <c r="D4" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="46" t="str">
         <f>Nifty!H4</f>
         <v>Net Profit</v>
       </c>
       <c r="I4" s="6">
         <f>Nifty!I4</f>
-        <v>19623.499999999909</v>
+        <v>-3696.7500000000045</v>
       </c>
       <c r="J4" s="5" t="str">
         <f>Nifty!J4</f>
@@ -3400,10 +3474,10 @@
       </c>
       <c r="K4" s="45">
         <f>Nifty!K4</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="L4" s="65">
-        <v>83200</v>
+        <v>82100</v>
       </c>
       <c r="M4" s="12">
         <v>6867</v>
@@ -3415,8 +3489,8 @@
         <v>13739</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="78"/>
       <c r="B5" s="51" t="s">
         <v>2</v>
       </c>
@@ -3426,18 +3500,18 @@
       <c r="D5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="124"/>
-      <c r="G5" s="108"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="44" t="str">
         <f>Nifty!H5</f>
         <v>Points</v>
       </c>
       <c r="I5" s="4">
         <f>Nifty!I5</f>
-        <v>16.899999999999949</v>
+        <v>12.25</v>
       </c>
       <c r="J5" s="5" t="str">
         <f>Nifty!J5</f>
@@ -3445,10 +3519,10 @@
       </c>
       <c r="K5" s="48">
         <f>Nifty!K5</f>
-        <v>0.78259999999999996</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="L5" s="65">
-        <v>83300</v>
+        <v>82200</v>
       </c>
       <c r="M5" s="20">
         <f>M4*$C$3</f>
@@ -3463,13 +3537,13 @@
         <v>13739</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="78"/>
       <c r="B6" s="50">
         <v>353.1</v>
       </c>
       <c r="C6" s="52">
-        <v>83600</v>
+        <v>82000</v>
       </c>
       <c r="D6" s="39">
         <v>309.5</v>
@@ -3479,24 +3553,24 @@
       </c>
       <c r="F6" s="38">
         <f>B6-D6+C6</f>
-        <v>83643.600000000006</v>
-      </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="84" t="str">
+        <v>82043.600000000006</v>
+      </c>
+      <c r="G6" s="112"/>
+      <c r="H6" s="88" t="str">
         <f>Nifty!H6</f>
         <v>Positives &amp; Negatives</v>
       </c>
-      <c r="I6" s="85"/>
+      <c r="I6" s="89"/>
       <c r="J6" s="63">
         <f>Nifty!J6</f>
-        <v>32295.749999999913</v>
+        <v>6459.4999999999845</v>
       </c>
       <c r="K6" s="64">
         <f>Nifty!K6</f>
-        <v>-12672.250000000005</v>
+        <v>-10156.249999999989</v>
       </c>
       <c r="L6" s="65">
-        <v>83400</v>
+        <v>82300</v>
       </c>
       <c r="M6" s="15">
         <v>-36</v>
@@ -3508,8 +3582,8 @@
         <v>-72</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="78"/>
       <c r="B7" s="53">
         <v>0</v>
       </c>
@@ -3519,35 +3593,35 @@
       <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="106" t="s">
+      <c r="E7" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="107"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="103" t="s">
+      <c r="F7" s="111"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="105"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="109"/>
       <c r="L7" s="65">
-        <v>83500</v>
-      </c>
-      <c r="M7" s="125" t="s">
+        <v>82400</v>
+      </c>
+      <c r="M7" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="126"/>
-      <c r="O7" s="127"/>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="121"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="103"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="78"/>
       <c r="B8" s="57" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="96" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="27" t="s">
@@ -3556,19 +3630,19 @@
       <c r="F8" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="108"/>
+      <c r="G8" s="112"/>
       <c r="H8" s="44" t="s">
         <v>22</v>
       </c>
       <c r="I8" s="8">
         <v>2</v>
       </c>
-      <c r="J8" s="102" t="s">
+      <c r="J8" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="100"/>
+      <c r="K8" s="104"/>
       <c r="L8" s="65">
-        <v>83600</v>
+        <v>82500</v>
       </c>
       <c r="M8" s="10" t="s">
         <v>2</v>
@@ -3580,32 +3654,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A9" s="78"/>
       <c r="B9" s="59" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="93"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="70" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="71">
         <v>2</v>
       </c>
-      <c r="G9" s="108"/>
+      <c r="G9" s="112"/>
       <c r="H9" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="8">
         <v>0</v>
       </c>
-      <c r="J9" s="102"/>
-      <c r="K9" s="100"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="104"/>
       <c r="L9" s="65">
-        <v>83700</v>
+        <v>82600</v>
       </c>
       <c r="M9" s="12">
         <v>189641.83999999997</v>
@@ -3617,30 +3691,30 @@
         <v>223923.83999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="78"/>
       <c r="B10" s="59" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="93"/>
+      <c r="D10" s="97"/>
       <c r="E10" s="29" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="108"/>
-      <c r="H10" s="129" t="s">
+      <c r="G10" s="112"/>
+      <c r="H10" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="117"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="74"/>
       <c r="L10" s="65">
-        <v>83800</v>
+        <v>82700</v>
       </c>
       <c r="M10" s="23">
         <f>M9*$C$3</f>
@@ -3655,22 +3729,22 @@
         <v>223923.83999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="78"/>
       <c r="B11" s="59" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="31" t="s">
         <v>67</v>
       </c>
       <c r="F11" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="108"/>
+      <c r="G11" s="112"/>
       <c r="H11" s="10">
         <v>0</v>
       </c>
@@ -3680,34 +3754,34 @@
       <c r="J11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="100" t="s">
+      <c r="K11" s="104" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="65">
-        <v>83900</v>
-      </c>
-      <c r="M11" s="89" t="s">
+        <v>82800</v>
+      </c>
+      <c r="M11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="90"/>
-      <c r="O11" s="91"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="121"/>
+      <c r="N11" s="94"/>
+      <c r="O11" s="95"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A12" s="78"/>
       <c r="B12" s="59" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="93"/>
+      <c r="D12" s="97"/>
       <c r="E12" s="31" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="108"/>
+      <c r="G12" s="112"/>
       <c r="H12" s="44" t="s">
         <v>28</v>
       </c>
@@ -3717,32 +3791,32 @@
       <c r="J12" s="8">
         <v>0</v>
       </c>
-      <c r="K12" s="100"/>
+      <c r="K12" s="104"/>
       <c r="L12" s="65">
-        <v>84000</v>
-      </c>
-      <c r="M12" s="128" t="s">
+        <v>82900</v>
+      </c>
+      <c r="M12" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="N12" s="110"/>
-      <c r="O12" s="111"/>
-    </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="122"/>
+      <c r="N12" s="114"/>
+      <c r="O12" s="115"/>
+    </row>
+    <row r="13" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="79"/>
       <c r="B13" s="61" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="94"/>
+      <c r="D13" s="98"/>
       <c r="E13" s="35" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="88"/>
+      <c r="G13" s="92"/>
       <c r="H13" s="47" t="s">
         <v>29</v>
       </c>
@@ -3752,35 +3826,35 @@
       <c r="J13" s="33">
         <v>0</v>
       </c>
-      <c r="K13" s="101"/>
+      <c r="K13" s="105"/>
       <c r="L13" s="66">
-        <v>84100</v>
-      </c>
-      <c r="M13" s="112"/>
-      <c r="N13" s="113"/>
-      <c r="O13" s="114"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="86">
+        <v>83000</v>
+      </c>
+      <c r="M13" s="116"/>
+      <c r="N13" s="117"/>
+      <c r="O13" s="118"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="90">
         <v>62.09</v>
       </c>
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
+      <c r="O14" s="92"/>
       <c r="P14" s="19"/>
     </row>
-    <row r="15" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -3821,7 +3895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3865,7 +3939,7 @@
         <v>-54</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3876,7 +3950,7 @@
         <v>-8.7099999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3887,19 +3961,15 @@
         <v>620</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.5">
       <c r="J19" s="3"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.5">
       <c r="L21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J8:K9"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="M12:O13"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="D3:F3"/>
@@ -3916,6 +3986,10 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="H1:O1"/>
     <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J8:K9"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="M12:O13"/>
   </mergeCells>
   <conditionalFormatting sqref="K16:N16 N17">
     <cfRule type="cellIs" dxfId="3" priority="7" operator="lessThan">

</xml_diff>